<commit_message>
Update Pinlayout spreadsheet with keypad pin mapping
</commit_message>
<xml_diff>
--- a/project/PinLayout.xlsx
+++ b/project/PinLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MicroP\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\School\ECSE 426\Lab Code\MicroP\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="53">
   <si>
     <t>PORT</t>
   </si>
@@ -160,6 +160,30 @@
   </si>
   <si>
     <t>TIM2 is reserved for interrupt</t>
+  </si>
+  <si>
+    <t>Keypad Pin 5</t>
+  </si>
+  <si>
+    <t>Keypad Pin 6</t>
+  </si>
+  <si>
+    <t>Keypad Pin 7</t>
+  </si>
+  <si>
+    <t>Keypad Pin 8</t>
+  </si>
+  <si>
+    <t>Keypad Pin 1</t>
+  </si>
+  <si>
+    <t>Keypad Pin 2</t>
+  </si>
+  <si>
+    <t>Keypad Pin 3</t>
+  </si>
+  <si>
+    <t>Keypad Pin 4</t>
   </si>
 </sst>
 </file>
@@ -522,8 +546,8 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1064,9 @@
       <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1058,7 +1084,9 @@
       <c r="F22" s="3">
         <v>3</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1108,7 +1136,9 @@
       <c r="F25" s="3">
         <v>6</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -1124,7 +1154,9 @@
       <c r="F26" s="3">
         <v>7</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -1140,7 +1172,9 @@
       <c r="F27" s="3">
         <v>8</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -1156,7 +1190,9 @@
       <c r="F28" s="3">
         <v>9</v>
       </c>
-      <c r="G28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -1172,7 +1208,9 @@
       <c r="F29" s="3">
         <v>10</v>
       </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -1190,7 +1228,9 @@
       <c r="F30" s="3">
         <v>11</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">

</xml_diff>

<commit_message>
Started working on interrupts for wireless
</commit_message>
<xml_diff>
--- a/project/PinLayout.xlsx
+++ b/project/PinLayout.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\School\ECSE 426\Lab Code\MicroP\project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Sender" sheetId="3" r:id="rId1"/>
     <sheet name="Receiver" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="54">
   <si>
     <t>PORT</t>
   </si>
@@ -150,9 +145,6 @@
     <t>CC2500_SPI_NSS</t>
   </si>
   <si>
-    <t>CC2500 GDI0</t>
-  </si>
-  <si>
     <t>Motor Pitch TIM9_CH1</t>
   </si>
   <si>
@@ -184,13 +176,19 @@
   </si>
   <si>
     <t>Keypad Pin 4</t>
+  </si>
+  <si>
+    <t>CC2500_GDIO2</t>
+  </si>
+  <si>
+    <t>CC2500 GDIO0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,7 +321,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,7 +356,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,22 +533,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
@@ -565,7 +563,7 @@
     <col min="11" max="11" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -596,7 +594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -623,7 +621,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -648,7 +646,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -673,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -698,7 +696,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -723,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -750,7 +748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -777,7 +775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -804,7 +802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -829,7 +827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -856,7 +854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -881,7 +879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -906,7 +904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -931,7 +929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -958,7 +956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -985,7 +983,7 @@
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1008,7 @@
       </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="E18" s="1"/>
@@ -1018,7 +1016,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -1034,7 +1032,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
@@ -1050,7 +1048,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
@@ -1065,10 +1063,10 @@
         <v>2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
@@ -1085,10 +1083,10 @@
         <v>3</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1102,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -1122,7 +1120,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -1137,10 +1135,10 @@
         <v>6</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
@@ -1155,10 +1153,10 @@
         <v>7</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="3" t="s">
         <v>3</v>
       </c>
@@ -1173,10 +1171,10 @@
         <v>8</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
@@ -1191,17 +1189,19 @@
         <v>9</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="3">
         <v>10</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>5</v>
       </c>
@@ -1209,10 +1209,10 @@
         <v>10</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>11</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>5</v>
@@ -1229,10 +1229,10 @@
         <v>11</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
@@ -1319,15 +1319,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
@@ -1342,7 +1342,7 @@
     <col min="11" max="11" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>6</v>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="E18" s="1"/>
@@ -1777,7 +1777,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
@@ -1825,10 +1825,10 @@
       </c>
       <c r="G21" s="4"/>
       <c r="K21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -1862,7 +1862,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3" t="s">
         <v>3</v>
       </c>
@@ -1928,7 +1928,7 @@
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
@@ -1944,14 +1944,16 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="3">
         <v>10</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>5</v>
       </c>
@@ -1960,14 +1962,16 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="3">
         <v>11</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="E30" s="3" t="s">
         <v>5</v>
       </c>
@@ -1976,14 +1980,16 @@
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="3">
         <v>12</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E31" s="3" t="s">
         <v>5</v>
       </c>
@@ -1994,14 +2000,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="3">
         <v>13</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E32" s="3" t="s">
         <v>5</v>
       </c>
@@ -2012,14 +2020,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="3">
         <v>14</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="E33" s="3" t="s">
         <v>5</v>
       </c>
@@ -2030,14 +2040,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="3">
         <v>15</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="E34" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>